<commit_message>
Nuevas pruebas de rendimiento
</commit_message>
<xml_diff>
--- a/src/performance/petclinic-performance.xlsx
+++ b/src/performance/petclinic-performance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Ruano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Ruano\eclipse-workspace\DP2-G7\src\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC57B08-1D4C-4A82-8444-B65F4DE75F85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626F77C9-EB6C-427B-A2C2-D212B0D1BB11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{C9C92E9B-5B3A-455A-B115-9EAA91F4BA51}"/>
+    <workbookView xWindow="5895" yWindow="3540" windowWidth="21600" windowHeight="11385" xr2:uid="{C9C92E9B-5B3A-455A-B115-9EAA91F4BA51}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Óptimo</t>
   </si>
   <si>
-    <t>Mínimo Ruputra</t>
-  </si>
-  <si>
     <t>ConcertarCita</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>BajaMascota</t>
+  </si>
+  <si>
+    <t>Mínimo Ruptura</t>
   </si>
 </sst>
 </file>
@@ -93,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +112,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -125,10 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +453,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,72 +470,87 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" s="1">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="B11" s="1">
+        <v>2600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edición de excel performance
</commit_message>
<xml_diff>
--- a/src/performance/petclinic-performance.xlsx
+++ b/src/performance/petclinic-performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Ruano\eclipse-workspace\DP2-G7\src\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D25348A-CC3E-4FC2-8AA0-3ADB98C35D37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC2EFFB-D0E9-4A5A-80EC-7B3FB53903D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5895" yWindow="1905" windowWidth="21600" windowHeight="13320" xr2:uid="{C9C92E9B-5B3A-455A-B115-9EAA91F4BA51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Historia de usuario</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Profiling</t>
-  </si>
-  <si>
-    <t>Profiling?</t>
   </si>
   <si>
     <t>ActualizarPruebasMedicas</t>
@@ -221,13 +218,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +543,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,8 +611,8 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -628,9 +626,6 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -722,7 +717,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>500</v>
@@ -755,7 +750,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>100</v>
@@ -769,7 +764,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>100</v>
@@ -777,13 +772,11 @@
       <c r="C19" s="3">
         <v>1500</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>200</v>
@@ -794,7 +787,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>1500</v>
@@ -805,7 +798,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>300</v>
@@ -813,13 +806,10 @@
       <c r="C22" s="3">
         <v>2500</v>
       </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>300</v>
@@ -827,13 +817,10 @@
       <c r="C23" s="3">
         <v>2500</v>
       </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>3000</v>
@@ -844,7 +831,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
         <v>50</v>
@@ -852,13 +839,11 @@
       <c r="C25" s="3">
         <v>300</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>10</v>
@@ -872,7 +857,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>5000</v>
@@ -883,7 +868,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1">
         <v>4000</v>
@@ -894,7 +879,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1">
         <v>150</v>
@@ -902,22 +887,19 @@
       <c r="C29" s="3">
         <v>1000</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
         <v>150</v>
       </c>
       <c r="C30" s="3">
         <v>1000</v>
-      </c>
-      <c r="E30" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>